<commit_message>
setting up models, templates and views
</commit_message>
<xml_diff>
--- a/valid_excel.xlsx
+++ b/valid_excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>FIRST NAME</t>
   </si>
@@ -34,58 +34,13 @@
     <t>SALARY</t>
   </si>
   <si>
-    <t>Testing</t>
+    <t>ATOBRAL</t>
   </si>
   <si>
-    <t>One</t>
-  </si>
-  <si>
-    <t>"2022-03-22"</t>
+    <t>Gideon</t>
   </si>
   <si>
     <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>Two</t>
-  </si>
-  <si>
-    <t>"2022-03-23"</t>
-  </si>
-  <si>
-    <t>Product Manager</t>
-  </si>
-  <si>
-    <t>Three</t>
-  </si>
-  <si>
-    <t>"2022-03-24"</t>
-  </si>
-  <si>
-    <t>Computer Engineer</t>
-  </si>
-  <si>
-    <t>Four</t>
-  </si>
-  <si>
-    <t>"2022-03-25"</t>
-  </si>
-  <si>
-    <t>Mobile Developer</t>
-  </si>
-  <si>
-    <t>Five</t>
-  </si>
-  <si>
-    <t>"2022-03-26"</t>
-  </si>
-  <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>"2022-03-27"</t>
-  </si>
-  <si>
-    <t>"2022-03-28"</t>
   </si>
 </sst>
 </file>
@@ -1036,13 +991,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15.75" outlineLevelRow="7" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="17.86" customWidth="1"/>
     <col min="2" max="2" width="18.7133333333333" customWidth="1"/>
@@ -1081,139 +1036,48 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>44637</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44638</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>200</v>
-      </c>
+    <row r="3" spans="3:7">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
-      </c>
+    <row r="4" spans="3:7">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5">
-        <v>500</v>
-      </c>
+    <row r="5" spans="7:7">
+      <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6">
-        <v>700</v>
-      </c>
+    <row r="6" spans="7:7">
+      <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7">
-        <v>700</v>
-      </c>
+    <row r="7" spans="7:7">
+      <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>500</v>
-      </c>
+    <row r="8" spans="7:7">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="7:7">
+      <c r="G9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>